<commit_message>
updated search option in alumni
</commit_message>
<xml_diff>
--- a/Excel/BSC_ComputerScience.xlsx
+++ b/Excel/BSC_ComputerScience.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Shivani Sharma</t>
   </si>
@@ -87,6 +87,9 @@
       </rPr>
       <t>Vijay Patidar</t>
     </r>
+  </si>
+  <si>
+    <t>Kanhapatidar@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -116,17 +119,18 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9A0004"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -244,8 +248,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -270,9 +275,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -285,8 +287,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,17 +631,17 @@
       <c r="D1" s="3">
         <v>8827578563</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -650,17 +656,17 @@
       <c r="D2" s="6">
         <v>8827742781</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -675,17 +681,17 @@
       <c r="D3" s="6">
         <v>8871739983</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -700,17 +706,17 @@
       <c r="D4" s="6">
         <v>7566983581</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -725,17 +731,17 @@
       <c r="D5" s="6">
         <v>8982127643</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -750,17 +756,17 @@
       <c r="D6" s="6">
         <v>7440507114</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -775,43 +781,49 @@
       <c r="D7" s="6">
         <v>9009618438</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="5">
         <v>2016</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="6">
         <v>9630046143</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="E7:F7"/>
@@ -824,10 +836,6 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" display="mailto:shivaniindore24@gmail.com"/>
@@ -837,6 +845,7 @@
     <hyperlink ref="C5" r:id="rId5" display="mailto:namangupta2406@gmail.com"/>
     <hyperlink ref="C6" r:id="rId6" display="mailto:admission@svvv.edu.in"/>
     <hyperlink ref="C7" r:id="rId7" display="mailto:gpatidar636@gmail.com"/>
+    <hyperlink ref="C8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>